<commit_message>
fix bug in user_list_template.xlsx && add doing next if job_num is empty
</commit_message>
<xml_diff>
--- a/用户信息上传模板.xlsx
+++ b/用户信息上传模板.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mushu/Desktop/电子中层干部考核/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mushu/rails/middle_manager_evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29560" yWindow="-19940" windowWidth="28040" windowHeight="17540"/>
+    <workbookView xWindow="28800" yWindow="-19940" windowWidth="21600" windowHeight="37940"/>
   </bookViews>
   <sheets>
     <sheet name="在职" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>序号</t>
   </si>
@@ -105,6 +105,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>7</t>
     </r>
@@ -113,6 +115,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>.1任电子工程系主任助理
 沪电信职院（2009）2号文2009.1.7任电子工程系主任助理
@@ -124,6 +128,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>）</t>
     </r>
@@ -132,6 +138,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>24</t>
     </r>
@@ -140,6 +148,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>号文</t>
     </r>
@@ -148,6 +158,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>2011.3.28</t>
     </r>
@@ -156,6 +168,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>任电子工程系副主任
 沪电信职院（</t>
@@ -165,6 +179,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>2013）8号文2013.2.1任电子工程系主任
 沪电信职院（</t>
@@ -174,6 +190,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>2015）10号文2015.4.8任电子工程系主任</t>
     </r>
@@ -211,17 +229,6 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>职工</t>
-    <rPh sb="0" eb="1">
-      <t>zhi'gong</t>
-    </rPh>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>66666666</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
     <t>我是领导</t>
     <rPh sb="0" eb="1">
       <t>wo'shi</t>
@@ -250,9 +257,6 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>1998/8</t>
-  </si>
-  <si>
     <t>工号*</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
@@ -276,10 +280,6 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>55555555</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
     <t>我是职工</t>
     <rPh sb="0" eb="1">
       <t>wo'shi</t>
@@ -336,9 +336,6 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>1998/9</t>
-  </si>
-  <si>
     <r>
       <t>沪电信职院（2009）2号文2009.1.7任图文信息中心主任助理
 沪电信职院（2010）53号文2010.7.29任图文信息中心副主任
@@ -349,6 +346,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>）</t>
     </r>
@@ -357,6 +356,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>24</t>
     </r>
@@ -365,6 +366,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>号文</t>
     </r>
@@ -373,6 +376,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>2011.3.28</t>
     </r>
@@ -381,6 +386,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>任图文信息中心副主任
 沪电信职院（</t>
@@ -390,6 +397,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>2013</t>
     </r>
@@ -398,6 +407,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>）</t>
     </r>
@@ -406,6 +417,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>8</t>
     </r>
@@ -414,6 +427,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>号文</t>
     </r>
@@ -422,6 +437,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>2013.2.1</t>
     </r>
@@ -430,6 +447,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>任图文信息中心副主任
 沪电信职院（2015）10号文2015.4.9任信息中心副主任</t>
@@ -457,6 +476,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>）</t>
     </r>
@@ -465,6 +486,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>24</t>
     </r>
@@ -473,6 +496,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>号文</t>
     </r>
@@ -481,6 +506,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>2011.3.28</t>
     </r>
@@ -489,6 +516,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>任图文信息中心副主任
 沪电信职院（</t>
@@ -498,6 +527,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>2013</t>
     </r>
@@ -506,6 +537,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>）</t>
     </r>
@@ -514,6 +547,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>8</t>
     </r>
@@ -522,6 +557,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>号文</t>
     </r>
@@ -530,6 +567,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>2013.2.1</t>
     </r>
@@ -538,6 +577,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
       </rPr>
       <t>任图文信息中心副主任
 沪电信职院（2015）10号文2015.4.10任信息中心副主任</t>
@@ -553,16 +594,6 @@
       </rPr>
       <t/>
     </r>
-  </si>
-  <si>
-    <t>职工职务</t>
-    <rPh sb="0" eb="1">
-      <t>zhi'gong</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>zhi'wu</t>
-    </rPh>
-    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>领导职务</t>
@@ -575,23 +606,6 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>77777777</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>我是中层干部</t>
-    <rPh sb="0" eb="1">
-      <t>wo'shi</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>zhong'c</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>gan'bu</t>
-    </rPh>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
     <t>学  院  干  部  基  本  信  息  表 （ 带 * 号项 必填，仅支持xlsx格式文件）</t>
     <rPh sb="28" eb="29">
       <t>dai</t>
@@ -616,6 +630,29 @@
     </rPh>
     <rPh sb="47" eb="48">
       <t>wen'jian</t>
+    </rPh>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>1990/8</t>
+  </si>
+  <si>
+    <t>1990/9</t>
+  </si>
+  <si>
+    <t>我是中层</t>
+    <rPh sb="0" eb="1">
+      <t>wo'shi</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>zhong'c</t>
+    </rPh>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>职工</t>
+    <rPh sb="0" eb="1">
+      <t>zhi'gog</t>
     </rPh>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
@@ -647,16 +684,22 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="华文宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
@@ -668,6 +711,8 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -680,6 +725,8 @@
       <sz val="24"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
@@ -738,7 +785,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -755,25 +802,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -803,8 +838,30 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1115,36 +1172,36 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4" style="10" customWidth="1"/>
+    <col min="1" max="1" width="4" style="7" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="14.5" style="10" customWidth="1"/>
-    <col min="5" max="5" width="3.33203125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="6" style="14" customWidth="1"/>
-    <col min="7" max="7" width="17.5" style="10" customWidth="1"/>
+    <col min="3" max="4" width="14.5" style="7" customWidth="1"/>
+    <col min="5" max="5" width="3.33203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="6" style="10" customWidth="1"/>
+    <col min="7" max="7" width="17.5" style="7" customWidth="1"/>
     <col min="8" max="8" width="3.83203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.1640625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="7.1640625" style="10" customWidth="1"/>
-    <col min="12" max="13" width="8.6640625" style="14" customWidth="1"/>
-    <col min="14" max="14" width="11" style="10" customWidth="1"/>
-    <col min="15" max="15" width="14.6640625" style="10" customWidth="1"/>
-    <col min="16" max="16" width="13" style="10" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" style="10" customWidth="1"/>
-    <col min="18" max="18" width="8.1640625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" style="7" customWidth="1"/>
+    <col min="12" max="13" width="8.6640625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="11" style="7" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="13" style="7" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" style="7" customWidth="1"/>
+    <col min="18" max="18" width="8.1640625" style="7" customWidth="1"/>
     <col min="19" max="19" width="72.6640625" style="2" customWidth="1"/>
     <col min="20" max="20" width="31.6640625" style="2" customWidth="1"/>
-    <col min="21" max="21" width="15.1640625" style="10" customWidth="1"/>
+    <col min="21" max="21" width="15.1640625" style="7" customWidth="1"/>
     <col min="22" max="22" width="45.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -1167,113 +1224,113 @@
       <c r="T1" s="22"/>
       <c r="U1" s="22"/>
     </row>
-    <row r="3" spans="1:22" s="18" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:22" s="14" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="G3" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="17" t="s">
+      <c r="H3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="15" t="s">
+      <c r="R3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="V3" s="18" t="s">
         <v>45</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="N3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="O3" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="P3" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q3" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="R3" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="S3" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="T3" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="U3" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="V3" s="18" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:22" s="2" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>55</v>
+      <c r="B4" s="25">
+        <v>77777777</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="17" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="8">
         <v>25159</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="9">
         <f t="shared" ref="H4" ca="1" si="0">YEAR(TODAY())-YEAR(G4)</f>
         <v>48</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="6" t="s">
         <v>15</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="M4" s="15" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="5" t="s">
@@ -1282,24 +1339,24 @@
       <c r="O4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="12" t="s">
+      <c r="P4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="Q4" s="11">
+      <c r="Q4" s="8">
         <v>41306</v>
       </c>
-      <c r="R4" s="13">
+      <c r="R4" s="9">
         <f ca="1">YEAR(TODAY())-YEAR(Q4)</f>
         <v>3</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="S4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="T4" s="17" t="s">
         <v>23</v>
       </c>
       <c r="U4" s="3"/>
-      <c r="V4" s="2" t="s">
+      <c r="V4" s="23" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1307,1096 +1364,1102 @@
       <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="26">
+        <v>66666666</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="E5" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="F5" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="11">
+      <c r="G5" s="8">
         <v>28230</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="19">
         <f t="shared" ref="H5:H6" ca="1" si="1">YEAR(TODAY())-YEAR(G5)</f>
         <v>39</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="17" t="s">
         <v>15</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L5" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="M5" s="15" t="s">
         <v>25</v>
       </c>
       <c r="N5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="21" t="s">
+      <c r="O5" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="P5" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q5" s="11">
+      <c r="P5" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q5" s="8">
         <v>42103</v>
       </c>
-      <c r="R5" s="13">
+      <c r="R5" s="9">
         <f ca="1">YEAR(TODAY())-YEAR(Q5)</f>
         <v>1</v>
       </c>
-      <c r="S5" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="U5" s="10"/>
-      <c r="V5" t="s">
+      <c r="S5" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="T5" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="U5" s="20"/>
+      <c r="V5" s="24" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="26">
+        <v>55555555</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="11">
+      <c r="G6" s="8">
         <v>28231</v>
       </c>
-      <c r="H6" s="2">
-        <f t="shared" ca="1" si="1"/>
+      <c r="H6" s="19">
+        <f t="shared" ref="H6" ca="1" si="2">YEAR(TODAY())-YEAR(G6)</f>
         <v>39</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="J6" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="17" t="s">
         <v>15</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="L6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="M6" s="19" t="s">
+      <c r="M6" s="15" t="s">
         <v>25</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O6" s="21" t="s">
+      <c r="O6" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="P6" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q6" s="11">
+      <c r="P6" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q6" s="8">
         <v>42104</v>
       </c>
-      <c r="R6" s="13">
+      <c r="R6" s="9">
         <f ca="1">YEAR(TODAY())-YEAR(Q6)</f>
         <v>1</v>
       </c>
-      <c r="S6" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="U6" s="10"/>
-      <c r="V6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" s="2" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S6" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="T6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="U6" s="20"/>
+      <c r="V6" s="24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="U7" s="10"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="U7" s="7"/>
       <c r="V7"/>
     </row>
     <row r="8" spans="1:22" s="2" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="U8" s="10"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="U8" s="7"/>
       <c r="V8"/>
     </row>
     <row r="9" spans="1:22" s="2" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="U9" s="10"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="U9" s="7"/>
       <c r="V9"/>
     </row>
     <row r="10" spans="1:22" s="2" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="U10" s="10"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="U10" s="7"/>
       <c r="V10"/>
     </row>
     <row r="11" spans="1:22" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="U11" s="10"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="U11" s="7"/>
       <c r="V11"/>
     </row>
     <row r="12" spans="1:22" s="2" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="U12" s="10"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="U12" s="7"/>
       <c r="V12"/>
     </row>
     <row r="13" spans="1:22" s="2" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="U13" s="10"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="U13" s="7"/>
       <c r="V13"/>
     </row>
     <row r="14" spans="1:22" s="2" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="U14" s="10"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="U14" s="7"/>
       <c r="V14"/>
     </row>
     <row r="15" spans="1:22" s="2" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="U15" s="10"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="U15" s="7"/>
       <c r="V15"/>
     </row>
     <row r="16" spans="1:22" s="2" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="U16" s="10"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="U16" s="7"/>
       <c r="V16"/>
     </row>
     <row r="17" spans="1:22" s="2" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="U17" s="10"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="U17" s="7"/>
       <c r="V17"/>
     </row>
     <row r="18" spans="1:22" s="2" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="U18" s="10"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="U18" s="7"/>
       <c r="V18"/>
     </row>
     <row r="19" spans="1:22" s="2" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="U19" s="10"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="U19" s="7"/>
       <c r="V19"/>
     </row>
     <row r="20" spans="1:22" s="2" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="U20" s="10"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="U20" s="7"/>
       <c r="V20"/>
     </row>
     <row r="21" spans="1:22" s="2" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="U21" s="10"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="U21" s="7"/>
       <c r="V21"/>
     </row>
     <row r="22" spans="1:22" s="2" customFormat="1" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="U22" s="10"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="U22" s="7"/>
       <c r="V22"/>
     </row>
     <row r="23" spans="1:22" s="2" customFormat="1" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="U23" s="10"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="U23" s="7"/>
       <c r="V23"/>
     </row>
     <row r="24" spans="1:22" s="2" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
-      <c r="U24" s="10"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="U24" s="7"/>
       <c r="V24"/>
     </row>
     <row r="25" spans="1:22" s="2" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
-      <c r="U25" s="10"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="U25" s="7"/>
       <c r="V25"/>
     </row>
     <row r="26" spans="1:22" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="10"/>
-      <c r="U26" s="10"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="U26" s="7"/>
       <c r="V26"/>
     </row>
     <row r="27" spans="1:22" s="2" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
-      <c r="U27" s="10"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="U27" s="7"/>
       <c r="V27"/>
     </row>
     <row r="28" spans="1:22" s="2" customFormat="1" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10"/>
-      <c r="U28" s="10"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="U28" s="7"/>
       <c r="V28"/>
     </row>
     <row r="29" spans="1:22" s="2" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="10"/>
-      <c r="U29" s="10"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="U29" s="7"/>
       <c r="V29"/>
     </row>
     <row r="30" spans="1:22" s="2" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="10"/>
-      <c r="U30" s="10"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="U30" s="7"/>
       <c r="V30"/>
     </row>
     <row r="31" spans="1:22" s="2" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
-      <c r="Q31" s="10"/>
-      <c r="R31" s="10"/>
-      <c r="U31" s="10"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="U31" s="7"/>
       <c r="V31"/>
     </row>
     <row r="32" spans="1:22" s="2" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="10"/>
-      <c r="R32" s="10"/>
-      <c r="U32" s="10"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="U32" s="7"/>
       <c r="V32"/>
     </row>
     <row r="33" spans="1:22" s="2" customFormat="1" ht="114" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="10"/>
-      <c r="R33" s="10"/>
-      <c r="U33" s="10"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="U33" s="7"/>
       <c r="V33"/>
     </row>
     <row r="34" spans="1:22" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="10"/>
-      <c r="U34" s="10"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="U34" s="7"/>
       <c r="V34"/>
     </row>
     <row r="35" spans="1:22" s="2" customFormat="1" ht="154" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
-      <c r="P35" s="10"/>
-      <c r="Q35" s="10"/>
-      <c r="R35" s="10"/>
-      <c r="U35" s="10"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="U35" s="7"/>
       <c r="V35"/>
     </row>
     <row r="36" spans="1:22" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="10"/>
-      <c r="O36" s="10"/>
-      <c r="P36" s="10"/>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="10"/>
-      <c r="U36" s="10"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="U36" s="7"/>
       <c r="V36"/>
     </row>
     <row r="37" spans="1:22" s="2" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="10"/>
-      <c r="P37" s="10"/>
-      <c r="Q37" s="10"/>
-      <c r="R37" s="10"/>
-      <c r="U37" s="10"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="U37" s="7"/>
       <c r="V37"/>
     </row>
     <row r="38" spans="1:22" s="2" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="10"/>
-      <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
-      <c r="Q38" s="10"/>
-      <c r="R38" s="10"/>
-      <c r="U38" s="10"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="U38" s="7"/>
       <c r="V38"/>
     </row>
     <row r="39" spans="1:22" s="2" customFormat="1" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="10"/>
-      <c r="U39" s="10"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="U39" s="7"/>
       <c r="V39"/>
     </row>
     <row r="40" spans="1:22" s="2" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
-      <c r="Q40" s="10"/>
-      <c r="R40" s="10"/>
-      <c r="U40" s="10"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="U40" s="7"/>
       <c r="V40"/>
     </row>
     <row r="41" spans="1:22" s="2" customFormat="1" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
-      <c r="P41" s="10"/>
-      <c r="Q41" s="10"/>
-      <c r="R41" s="10"/>
-      <c r="U41" s="10"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="U41" s="7"/>
       <c r="V41"/>
     </row>
     <row r="42" spans="1:22" s="2" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="10"/>
-      <c r="R42" s="10"/>
-      <c r="U42" s="10"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+      <c r="U42" s="7"/>
       <c r="V42"/>
     </row>
     <row r="43" spans="1:22" s="2" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="10"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10"/>
-      <c r="Q43" s="10"/>
-      <c r="R43" s="10"/>
-      <c r="U43" s="10"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
+      <c r="U43" s="7"/>
       <c r="V43"/>
     </row>
     <row r="44" spans="1:22" s="2" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="1"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="10"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="10"/>
-      <c r="K44" s="10"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="10"/>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="10"/>
-      <c r="R44" s="10"/>
-      <c r="U44" s="10"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
+      <c r="Q44" s="7"/>
+      <c r="R44" s="7"/>
+      <c r="U44" s="7"/>
       <c r="V44"/>
     </row>
     <row r="45" spans="1:22" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="10"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="10"/>
-      <c r="K45" s="10"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="10"/>
-      <c r="O45" s="10"/>
-      <c r="P45" s="10"/>
-      <c r="Q45" s="10"/>
-      <c r="R45" s="10"/>
-      <c r="U45" s="10"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="7"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
+      <c r="U45" s="7"/>
       <c r="V45"/>
     </row>
     <row r="46" spans="1:22" s="2" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="10"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="10"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="10"/>
-      <c r="O46" s="10"/>
-      <c r="P46" s="10"/>
-      <c r="Q46" s="10"/>
-      <c r="R46" s="10"/>
-      <c r="U46" s="10"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="7"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="7"/>
+      <c r="U46" s="7"/>
       <c r="V46"/>
     </row>
     <row r="47" spans="1:22" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="1"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="10"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="10"/>
-      <c r="K47" s="10"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
-      <c r="N47" s="10"/>
-      <c r="O47" s="10"/>
-      <c r="P47" s="10"/>
-      <c r="Q47" s="10"/>
-      <c r="R47" s="10"/>
-      <c r="U47" s="10"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
+      <c r="Q47" s="7"/>
+      <c r="R47" s="7"/>
+      <c r="U47" s="7"/>
       <c r="V47"/>
     </row>
     <row r="48" spans="1:22" s="2" customFormat="1" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="1"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="10"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="10"/>
-      <c r="O48" s="10"/>
-      <c r="P48" s="10"/>
-      <c r="Q48" s="10"/>
-      <c r="R48" s="10"/>
-      <c r="U48" s="10"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
+      <c r="Q48" s="7"/>
+      <c r="R48" s="7"/>
+      <c r="U48" s="7"/>
       <c r="V48"/>
     </row>
     <row r="49" spans="1:22" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="14"/>
-      <c r="N49" s="10"/>
-      <c r="O49" s="10"/>
-      <c r="P49" s="10"/>
-      <c r="Q49" s="10"/>
-      <c r="R49" s="10"/>
-      <c r="U49" s="10"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="7"/>
+      <c r="P49" s="7"/>
+      <c r="Q49" s="7"/>
+      <c r="R49" s="7"/>
+      <c r="U49" s="7"/>
       <c r="V49"/>
     </row>
     <row r="50" spans="1:22" s="2" customFormat="1" ht="154" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="10"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
-      <c r="N50" s="10"/>
-      <c r="O50" s="10"/>
-      <c r="P50" s="10"/>
-      <c r="Q50" s="10"/>
-      <c r="R50" s="10"/>
-      <c r="U50" s="10"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
+      <c r="U50" s="7"/>
       <c r="V50"/>
     </row>
     <row r="51" spans="1:22" s="2" customFormat="1" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="1"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="10"/>
-      <c r="I51" s="10"/>
-      <c r="J51" s="10"/>
-      <c r="K51" s="10"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="10"/>
-      <c r="O51" s="10"/>
-      <c r="P51" s="10"/>
-      <c r="Q51" s="10"/>
-      <c r="R51" s="10"/>
-      <c r="U51" s="10"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="10"/>
+      <c r="M51" s="10"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
+      <c r="P51" s="7"/>
+      <c r="Q51" s="7"/>
+      <c r="R51" s="7"/>
+      <c r="U51" s="7"/>
       <c r="V51"/>
     </row>
     <row r="52" spans="1:22" s="2" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3"/>
+      <c r="A52" s="7"/>
       <c r="B52" s="1"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="10"/>
-      <c r="I52" s="10"/>
-      <c r="J52" s="10"/>
-      <c r="K52" s="10"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="10"/>
-      <c r="O52" s="10"/>
-      <c r="P52" s="10"/>
-      <c r="Q52" s="10"/>
-      <c r="R52" s="10"/>
-      <c r="U52" s="10"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="7"/>
+      <c r="K52" s="7"/>
+      <c r="L52" s="10"/>
+      <c r="M52" s="10"/>
+      <c r="N52" s="7"/>
+      <c r="O52" s="7"/>
+      <c r="P52" s="7"/>
+      <c r="Q52" s="7"/>
+      <c r="R52" s="7"/>
+      <c r="U52" s="7"/>
       <c r="V52"/>
     </row>
     <row r="53" spans="1:22" ht="39" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>